<commit_message>
TestNG da test kiem thuư web
</commit_message>
<xml_diff>
--- a/HiNoApp/EXCEL_DIRSaveTestNGResultToExecl.xlsx
+++ b/HiNoApp/EXCEL_DIRSaveTestNGResultToExecl.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Test Step No.</t>
   </si>
@@ -44,28 +44,70 @@
     <t>1</t>
   </si>
   <si>
+    <t>Test Login susscess with valid username and password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Test Login fail with invalid username</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>Username : Admin</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>D:/3tProject-KiemThu/HiNoApp/Resources/image/failure1702106675928.png</t>
+  </si>
+  <si>
+    <t>full img</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Test Login fail with invalid password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Password : admin123</t>
+  </si>
+  <si>
+    <t>D:/3tProject-KiemThu/HiNoApp/Resources/image/failure1702106691537.png</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Test Login fail with invalid username and password</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>Dashboard4</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>D:/3tProject-KiemThu/HiNoApp/Resources/image/failure1701919458306.png</t>
-  </si>
-  <si>
-    <t>full img</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>D:/3tProject-KiemThu/HiNoApp/Resources/image/failure1702106705508.png</t>
   </si>
 </sst>
 </file>
@@ -102,13 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -119,13 +159,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -153,12 +193,88 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="533400" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="533400" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -193,7 +309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="80.0" customHeight="true">
+    <row r="2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -210,18 +326,98 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" ht="80.0" customHeight="true">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="80.0" customHeight="true">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="80.0" customHeight="true">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
+    <hyperlink ref="H5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>